<commit_message>
Added NOT_GIVEN_BIRTH state for negative rewarding on multiply failure
</commit_message>
<xml_diff>
--- a/Rewards.xlsx
+++ b/Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA - HungerStates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9D2E27-EFE4-4C4B-AF89-4D0AD50B8DF3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126A967-8B87-4442-9F32-ED658C9AC679}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17625" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>NO_FOOD</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>GIVEN_BIRTHFLEE</t>
+  </si>
+  <si>
+    <t>NOT_GIVEN_BIRTHRAND</t>
+  </si>
+  <si>
+    <t>NOT_GIVEN_BIRTHHUNT</t>
+  </si>
+  <si>
+    <t>NOT_GIVEN_BIRTHMULTIPLY</t>
+  </si>
+  <si>
+    <t>NOT_GIVEN_BIRTHFLEE</t>
+  </si>
+  <si>
+    <t>NOT_GIVEN_BIRTH</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -921,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H5" sqref="H5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,9 +951,10 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -948,8 +967,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -965,8 +987,11 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -982,8 +1007,11 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -999,8 +1027,11 @@
       <c r="E4" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1016,8 +1047,11 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1033,8 +1067,11 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1050,8 +1087,11 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1067,8 +1107,11 @@
       <c r="E8" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1084,8 +1127,11 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1101,8 +1147,11 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1118,8 +1167,11 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1135,8 +1187,11 @@
       <c r="E12" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1152,8 +1207,11 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1169,8 +1227,11 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1186,8 +1247,11 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1203,8 +1267,11 @@
       <c r="E16" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1219,6 +1286,89 @@
       </c>
       <c r="E17" s="1">
         <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>20</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>